<commit_message>
Fix Bug: Filter dropping no-redudant options
</commit_message>
<xml_diff>
--- a/Debugging Files/NBC_points.xlsx
+++ b/Debugging Files/NBC_points.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipeacevedo/Documents/Programing/controller_calculator-1/Debugging Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tranetechnologies-my.sharepoint.com/personal/felipe_acevedo_trane_com/Documents/Documents/Programming/controller_calculator/Debugging Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3661F7C0-9F43-C042-AB77-585BAAC6B14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{3661F7C0-9F43-C042-AB77-585BAAC6B14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C4149E5-B1DF-44FA-880B-CE818D67F69D}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="820" windowWidth="25820" windowHeight="17440" xr2:uid="{3685C660-8D48-5847-825B-DD00EC148610}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3685C660-8D48-5847-825B-DD00EC148610}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -485,15 +485,15 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -516,7 +516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -539,7 +539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -562,12 +562,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -585,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -602,13 +602,13 @@
         <v>6</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -631,7 +631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -648,18 +648,18 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -677,7 +677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Bug fixes, add GUI improvements, and implement tooltips for better user guidance.
</commit_message>
<xml_diff>
--- a/Debugging Files/NBC_points.xlsx
+++ b/Debugging Files/NBC_points.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tranetechnologies-my.sharepoint.com/personal/felipe_acevedo_trane_com/Documents/Documents/Programming/controller_calculator/Debugging Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipeacevedo/Documents/Programing/controller_calculator-1/Debugging Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{3661F7C0-9F43-C042-AB77-585BAAC6B14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C4149E5-B1DF-44FA-880B-CE818D67F69D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56693F7C-E179-D549-82D5-01E81D16DD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3685C660-8D48-5847-825B-DD00EC148610}"/>
+    <workbookView xWindow="4420" yWindow="640" windowWidth="25820" windowHeight="15720" xr2:uid="{3685C660-8D48-5847-825B-DD00EC148610}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -485,15 +485,15 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.875" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -516,7 +516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -539,7 +539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -562,7 +562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -585,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -608,7 +608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -631,7 +631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -654,12 +654,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -677,7 +677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>

</xml_diff>